<commit_message>
SSRT updated to exclude old programs
This update fixes an error where older versions of the program utilized the stop signal delay array in later versions as a holder for a different latency measure. A column has been added to the 'Group Identifier' spreadsheet in order to identify, and later ignore, these older programs.
</commit_message>
<xml_diff>
--- a/Group Identifier.xlsx
+++ b/Group Identifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stop Signal Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erikv\Desktop\SSRT Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B081CA5E-FE71-4699-87B8-0FAD5714FA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F6D69F-9A04-496B-AB0A-8F36A8E98835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26400" yWindow="3120" windowWidth="21600" windowHeight="11010" xr2:uid="{9FAA4369-990C-4EA5-9915-D7D26DB87606}"/>
+    <workbookView xWindow="5565" yWindow="2940" windowWidth="21705" windowHeight="15285" xr2:uid="{9FAA4369-990C-4EA5-9915-D7D26DB87606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Acceptable MSNs</t>
   </si>
   <si>
-    <t>Experimentals</t>
-  </si>
-  <si>
-    <t>Controls</t>
-  </si>
-  <si>
     <t>&lt;--- dictate what programs collect data in a similar way</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>MSxc</t>
+  </si>
+  <si>
+    <t>M2-4624</t>
+  </si>
+  <si>
+    <t>M2-4645</t>
+  </si>
+  <si>
+    <t>25P STOP LT 3 Greg ZD v3</t>
+  </si>
+  <si>
+    <t>M2-4670</t>
+  </si>
+  <si>
+    <t>M2-4626</t>
+  </si>
+  <si>
+    <t>25P STOP LT 3 Greg ZD BoxA2</t>
+  </si>
+  <si>
+    <t>M2-4780</t>
+  </si>
+  <si>
+    <t>M2-4600</t>
+  </si>
+  <si>
+    <t>25P STOP 200ms TEST Greg SSRT BoxA4 v2</t>
+  </si>
+  <si>
+    <t>M2-4795</t>
+  </si>
+  <si>
+    <t>M2-4599</t>
+  </si>
+  <si>
+    <t>25P STOP 50ms TEST Greg SSRT BoxA4 v2</t>
+  </si>
+  <si>
+    <t>M2-4860</t>
+  </si>
+  <si>
+    <t>M2-4874</t>
+  </si>
+  <si>
+    <t>25P STOP ZD TEST Greg SSRT BoxA4 v2</t>
+  </si>
+  <si>
+    <t>M2-4911</t>
+  </si>
+  <si>
+    <t>M2-4887</t>
+  </si>
+  <si>
+    <t>25P STOP Baseline Greg SSRT BoxA4 v2</t>
+  </si>
+  <si>
+    <t>M2-4861</t>
+  </si>
+  <si>
+    <t>M2-4886</t>
+  </si>
+  <si>
+    <t>25P STOP LT 3 Greg ZD v3 BoxA4</t>
+  </si>
+  <si>
+    <t>M2-4864</t>
+  </si>
+  <si>
+    <t>M2-4917</t>
+  </si>
+  <si>
+    <t>Lever Training 2 Greg</t>
+  </si>
+  <si>
+    <t>25P STOP 100ms TEST Greg SSRT BoxA2</t>
+  </si>
+  <si>
+    <t>25P STOP 300ms TEST Greg SSRT BoxA2</t>
+  </si>
+  <si>
+    <t>25P STOP Baseline Greg SSRT BoxA2 v2</t>
+  </si>
+  <si>
+    <t>Lever Training 2 Greg Box A2</t>
+  </si>
+  <si>
+    <t>Lever Training 1</t>
+  </si>
+  <si>
+    <t>LT 3 Greg ZD</t>
+  </si>
+  <si>
+    <t>LT 3 Greg ZD BoxA2</t>
+  </si>
+  <si>
+    <t>LT 3 Greg ZD BoxA4</t>
+  </si>
+  <si>
+    <t>Stop lever delay LT 3 Greg ZD v3</t>
+  </si>
+  <si>
+    <t>Stop lever delay LT 3 Greg ZD v3 A4</t>
+  </si>
+  <si>
+    <t>Stop lever delay LT 3 Greg ZD v3 A2</t>
+  </si>
+  <si>
+    <t>30sec pun LT 3 Greg ZD v3 BoxA2</t>
+  </si>
+  <si>
+    <t>30sec pun LT 3 Greg ZD v3</t>
+  </si>
+  <si>
+    <t>LT 3 ZD No Stop Lever BoxA4</t>
+  </si>
+  <si>
+    <t>LT 3 ZD No Stop Lever</t>
+  </si>
+  <si>
+    <t>LT 3 ZD No Stop Lever BoxA2</t>
+  </si>
+  <si>
+    <t>30sec pun LT 3 Greg ZD v3 BoxA4</t>
+  </si>
+  <si>
+    <t>Stop Lever Delay LT3 v1 Box A2</t>
+  </si>
+  <si>
+    <t>Stop Lever Delay LT3 v1</t>
+  </si>
+  <si>
+    <t>M2-4975</t>
+  </si>
+  <si>
+    <t>4911 Baseline SSRT BoxA2 v3</t>
+  </si>
+  <si>
+    <t>Do Not Parse for Test Breakdown</t>
   </si>
 </sst>
 </file>
@@ -406,31 +544,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF91D46-358B-454E-8E9A-8AF583BEEF68}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>